<commit_message>
Add updated and missing templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/DNA_extraction/DNA_extraction_v1.1.8.xlsx
+++ b/templates/dataplant/DNA_extraction/DNA_extraction_v1.1.8.xlsx
@@ -200,37 +200,37 @@
     <t/>
   </si>
   <si>
-    <t>total RNA</t>
-  </si>
-  <si>
-    <t>EFO</t>
-  </si>
-  <si>
-    <t>https://bioregistry.io/EFO:0004964</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>milligram</t>
+    <t>BAO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/BAO_0000269</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>gram</t>
   </si>
   <si>
     <t>UO</t>
   </si>
   <si>
-    <t>https://bioregistry.io/UO:0000022</t>
-  </si>
-  <si>
-    <t>QIAGEN RNEasy</t>
-  </si>
-  <si>
-    <t>QIAGEN RNEasy Buffer 2</t>
-  </si>
-  <si>
-    <t>microliter</t>
-  </si>
-  <si>
-    <t>https://bioregistry.io/UO:0000101</t>
+    <t>https://bioregistry.io/UO:0000021</t>
+  </si>
+  <si>
+    <t>Macherey Nagel NucleoBond HMW DNA Kit</t>
+  </si>
+  <si>
+    <t>Lysis buffer H1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>milliliter</t>
+  </si>
+  <si>
+    <t>https://bioregistry.io/UO:0000098</t>
   </si>
 </sst>
 </file>
@@ -888,28 +888,28 @@
         <v>61</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>65</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>66</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>67</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>68</v>
-      </c>
-      <c r="I2" t="s">
-        <v>69</v>
       </c>
       <c r="J2" t="s">
         <v>61</v>
@@ -918,7 +918,7 @@
         <v>61</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M2" t="s">
         <v>61</v>
@@ -927,13 +927,13 @@
         <v>61</v>
       </c>
       <c r="O2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="P2" t="s">
         <v>71</v>
       </c>
       <c r="Q2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R2" t="s">
         <v>72</v>

</xml_diff>